<commit_message>
Add car test firmware.
</commit_message>
<xml_diff>
--- a/Partslist.xlsx
+++ b/Partslist.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\landrygreg\Documents\Work_NextCloud\MIT\2022\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\landrygreg\Documents\Work_NextCloud\MIT\2022\BLE_Car_Git_Repo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4112E3EA-18ED-4973-97EF-77E6BBAA6835}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC53B1C9-B63D-42A7-9D59-54A66D01E752}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="14025" xr2:uid="{A224F4AB-A986-40DF-9520-9B2BF3357A4B}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Description</t>
   </si>
@@ -33,9 +33,6 @@
     <t>Item Link</t>
   </si>
   <si>
-    <t>Car kit</t>
-  </si>
-  <si>
     <t>Set of connector wires</t>
   </si>
   <si>
@@ -60,13 +57,13 @@
     <t>https://www.parallax.com/product/3v-digital-micro-servo-standard-ft90b/</t>
   </si>
   <si>
-    <t>https://stgrobotics.com/2019/01/15/vkmaker-new-avoidance-tracking-motor-smart-robot-car-chassis-kit-speed-encoder-battery-box-2wd-ultrasonic-module-with-tutorial-cd/</t>
-  </si>
-  <si>
-    <t>https://bulletinwave.com/2021/09/30/vkmaker-new-avoidance-tracking-motor-smart-robot-car-chassis-kit-speed-encoder-battery-box-2wd-ultrasonic-module-with-tutorial-cd/</t>
-  </si>
-  <si>
-    <t>https://www.walmart.ca/en/ip/VKmaker-New-Avoidance-tracking-Motor-Smart-Robot-Car-Chassis-Kit-Speed-Encoder-Battery-Box-2WD-Ultrasonic-module-with-tutorial/PRD5093WHPHLNAF</t>
+    <t>https://www.ebay.com/itm/403374607820?chn=ps&amp;norover=1&amp;mkevt=1&amp;mkrid=711-117182-37290-0&amp;mkcid=2&amp;itemid=403374607820&amp;targetid=1264870805664&amp;device=c&amp;mktype=pla&amp;googleloc=9002274&amp;poi=&amp;campaignid=13917919372&amp;mkgroupid=125280033815&amp;rlsatarget=pla-1264870805664&amp;abcId=9300614&amp;merchantid=101638797&amp;gclid=Cj0KCQiAw9qOBhC-ARIsAG-rdn418F73lj6LtbYeC-6c0Fu4bdQU6tLotSpCoHZtptx8vUXg1PcPYgUaAmDnEALw_wcB</t>
+  </si>
+  <si>
+    <t>Car kit *</t>
+  </si>
+  <si>
+    <t>* Note: if the car kit is not availble on the above link, search for "vkmaker new avoidance tracking motor smart robot car chassis kit"</t>
   </si>
 </sst>
 </file>
@@ -76,7 +73,7 @@
   <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -93,6 +90,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -129,9 +134,7 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="2" builtinId="4"/>
@@ -448,10 +451,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{476885E2-0F23-4E4E-9974-1DC60ADFF409}">
-  <dimension ref="A1:C21"/>
+  <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -465,7 +468,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -473,81 +476,78 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2">
+        <v>27.71</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3">
+        <v>6.99</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>2</v>
       </c>
-      <c r="B2">
-        <v>22.98</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C3" s="4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B4">
+        <v>6.98</v>
+      </c>
       <c r="C4" s="2" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B5">
-        <v>6.99</v>
+        <v>5.65</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>3</v>
-      </c>
-      <c r="B6">
-        <v>6.98</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7">
-        <v>5.65</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
+      </c>
+      <c r="B7" s="3">
+        <f>SUM(B2:B5)</f>
+        <v>47.330000000000005</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>8</v>
-      </c>
-      <c r="B9" s="3">
-        <f>SUM(B2:B7)</f>
-        <v>42.6</v>
-      </c>
-    </row>
-    <row r="21" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C21">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="4"/>
+    </row>
+    <row r="19" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C19">
         <f>26.88+4*6.99+6.98+42.83</f>
         <v>104.65</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C6" r:id="rId1" display="https://www.amazon.com/Elegoo-EL-CP-004-Multicolored-Breadboard-arduino/dp/B01EV70C78/ref=pd_bxgy_img_2/143-6431746-6933403?pd_rd_w=H22tl&amp;pf_rd_p=c64372fa-c41c-422e-990d-9e034f73989b&amp;pf_rd_r=J747F77KB86AZE8YJATE&amp;pd_rd_r=1f2016cb-91ff-4618-8f0c-c08e2b5a51cf&amp;pd_rd_wg=2mGQY&amp;pd_rd_i=B01EV70C78&amp;psc=1" xr:uid="{4229BFD4-19A3-4C5C-93B7-041B917B7132}"/>
-    <hyperlink ref="C5" r:id="rId2" display="https://www.amazon.com/Measuring-Optocoupler-Interrupter-Detection-Arduino%EF%BC%885pcs%EF%BC%89/dp/B08977QFK5/ref=pd_sbs_1/143-6431746-6933403?pd_rd_w=1rwuj&amp;pf_rd_p=0a3ad226-8a77-4898-9a99-63ffeb1aef90&amp;pf_rd_r=M16NNS5TBREKKMW088BK&amp;pd_rd_r=94423b03-ca05-44ab-b8e1-26aeb4d6030a&amp;pd_rd_wg=LJxVI&amp;pd_rd_i=B08977QFK5&amp;psc=1" xr:uid="{DDB4B196-43EA-4452-9352-4BB4E969990C}"/>
-    <hyperlink ref="C7" r:id="rId3" xr:uid="{4709149D-D041-4556-B5F5-7702278161E2}"/>
-    <hyperlink ref="C2" r:id="rId4" xr:uid="{EBB91B52-3735-46D1-9DC1-03EF9684D898}"/>
+    <hyperlink ref="C4" r:id="rId1" display="https://www.amazon.com/Elegoo-EL-CP-004-Multicolored-Breadboard-arduino/dp/B01EV70C78/ref=pd_bxgy_img_2/143-6431746-6933403?pd_rd_w=H22tl&amp;pf_rd_p=c64372fa-c41c-422e-990d-9e034f73989b&amp;pf_rd_r=J747F77KB86AZE8YJATE&amp;pd_rd_r=1f2016cb-91ff-4618-8f0c-c08e2b5a51cf&amp;pd_rd_wg=2mGQY&amp;pd_rd_i=B01EV70C78&amp;psc=1" xr:uid="{4229BFD4-19A3-4C5C-93B7-041B917B7132}"/>
+    <hyperlink ref="C3" r:id="rId2" display="https://www.amazon.com/Measuring-Optocoupler-Interrupter-Detection-Arduino%EF%BC%885pcs%EF%BC%89/dp/B08977QFK5/ref=pd_sbs_1/143-6431746-6933403?pd_rd_w=1rwuj&amp;pf_rd_p=0a3ad226-8a77-4898-9a99-63ffeb1aef90&amp;pf_rd_r=M16NNS5TBREKKMW088BK&amp;pd_rd_r=94423b03-ca05-44ab-b8e1-26aeb4d6030a&amp;pd_rd_wg=LJxVI&amp;pd_rd_i=B08977QFK5&amp;psc=1" xr:uid="{DDB4B196-43EA-4452-9352-4BB4E969990C}"/>
+    <hyperlink ref="C5" r:id="rId3" xr:uid="{4709149D-D041-4556-B5F5-7702278161E2}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId5"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add solution ModusToolbox project and Android app
</commit_message>
<xml_diff>
--- a/Partslist.xlsx
+++ b/Partslist.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20379"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20382"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\landrygreg\Documents\Work_NextCloud\MIT\2022\BLE_Car_Git_Repo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\landrygreg\Documents\Work_NextCloud\MIT\iap2022\BLE_Car_Git_Repo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC53B1C9-B63D-42A7-9D59-54A66D01E752}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD560AAB-B633-487F-BBC4-DFC1C1052189}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="14025" xr2:uid="{A224F4AB-A986-40DF-9520-9B2BF3357A4B}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="14030" xr2:uid="{A224F4AB-A986-40DF-9520-9B2BF3357A4B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Description</t>
   </si>
@@ -64,6 +64,12 @@
   </si>
   <si>
     <t>* Note: if the car kit is not availble on the above link, search for "vkmaker new avoidance tracking motor smart robot car chassis kit"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.infineon.com/cms/en/product/evaluation-boards/cy8ckit-062s2-43012 </t>
+  </si>
+  <si>
+    <t>PSoC 6 Wi-Fi/BLE kit</t>
   </si>
 </sst>
 </file>
@@ -451,19 +457,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{476885E2-0F23-4E4E-9974-1DC60ADFF409}">
-  <dimension ref="A1:C19"/>
+  <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="22.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="255.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.26953125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="255.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -474,80 +480,92 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2">
+        <v>122.43</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
         <v>11</v>
       </c>
-      <c r="B2">
+      <c r="B3">
         <v>27.71</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C3" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
         <v>3</v>
       </c>
-      <c r="B3">
+      <c r="B4">
         <v>6.99</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C4" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
         <v>2</v>
       </c>
-      <c r="B4">
+      <c r="B5">
         <v>6.98</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C5" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
         <v>8</v>
       </c>
-      <c r="B5">
+      <c r="B6">
         <v>5.65</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C6" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="3">
-        <f>SUM(B2:B5)</f>
-        <v>47.330000000000005</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="B8" s="3">
+        <f>SUM(B2:B6)</f>
+        <v>169.76000000000002</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="4"/>
-    </row>
-    <row r="19" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C19">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A11" s="4"/>
+    </row>
+    <row r="20" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C20">
         <f>26.88+4*6.99+6.98+42.83</f>
         <v>104.65</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C4" r:id="rId1" display="https://www.amazon.com/Elegoo-EL-CP-004-Multicolored-Breadboard-arduino/dp/B01EV70C78/ref=pd_bxgy_img_2/143-6431746-6933403?pd_rd_w=H22tl&amp;pf_rd_p=c64372fa-c41c-422e-990d-9e034f73989b&amp;pf_rd_r=J747F77KB86AZE8YJATE&amp;pd_rd_r=1f2016cb-91ff-4618-8f0c-c08e2b5a51cf&amp;pd_rd_wg=2mGQY&amp;pd_rd_i=B01EV70C78&amp;psc=1" xr:uid="{4229BFD4-19A3-4C5C-93B7-041B917B7132}"/>
-    <hyperlink ref="C3" r:id="rId2" display="https://www.amazon.com/Measuring-Optocoupler-Interrupter-Detection-Arduino%EF%BC%885pcs%EF%BC%89/dp/B08977QFK5/ref=pd_sbs_1/143-6431746-6933403?pd_rd_w=1rwuj&amp;pf_rd_p=0a3ad226-8a77-4898-9a99-63ffeb1aef90&amp;pf_rd_r=M16NNS5TBREKKMW088BK&amp;pd_rd_r=94423b03-ca05-44ab-b8e1-26aeb4d6030a&amp;pd_rd_wg=LJxVI&amp;pd_rd_i=B08977QFK5&amp;psc=1" xr:uid="{DDB4B196-43EA-4452-9352-4BB4E969990C}"/>
-    <hyperlink ref="C5" r:id="rId3" xr:uid="{4709149D-D041-4556-B5F5-7702278161E2}"/>
+    <hyperlink ref="C5" r:id="rId1" display="https://www.amazon.com/Elegoo-EL-CP-004-Multicolored-Breadboard-arduino/dp/B01EV70C78/ref=pd_bxgy_img_2/143-6431746-6933403?pd_rd_w=H22tl&amp;pf_rd_p=c64372fa-c41c-422e-990d-9e034f73989b&amp;pf_rd_r=J747F77KB86AZE8YJATE&amp;pd_rd_r=1f2016cb-91ff-4618-8f0c-c08e2b5a51cf&amp;pd_rd_wg=2mGQY&amp;pd_rd_i=B01EV70C78&amp;psc=1" xr:uid="{4229BFD4-19A3-4C5C-93B7-041B917B7132}"/>
+    <hyperlink ref="C4" r:id="rId2" display="https://www.amazon.com/Measuring-Optocoupler-Interrupter-Detection-Arduino%EF%BC%885pcs%EF%BC%89/dp/B08977QFK5/ref=pd_sbs_1/143-6431746-6933403?pd_rd_w=1rwuj&amp;pf_rd_p=0a3ad226-8a77-4898-9a99-63ffeb1aef90&amp;pf_rd_r=M16NNS5TBREKKMW088BK&amp;pd_rd_r=94423b03-ca05-44ab-b8e1-26aeb4d6030a&amp;pd_rd_wg=LJxVI&amp;pd_rd_i=B08977QFK5&amp;psc=1" xr:uid="{DDB4B196-43EA-4452-9352-4BB4E969990C}"/>
+    <hyperlink ref="C6" r:id="rId3" xr:uid="{4709149D-D041-4556-B5F5-7702278161E2}"/>
+    <hyperlink ref="C2" r:id="rId4" xr:uid="{36B4FB6C-4FEB-4A1B-A711-78A5618318EE}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId4"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>